<commit_message>
Creación de las consultas del cbr para determinar el destino del NPC
</commit_message>
<xml_diff>
--- a/cbr/modelo/speedcraft-casos.xlsx
+++ b/cbr/modelo/speedcraft-casos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="225" windowWidth="18915" windowHeight="8385" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="285" windowWidth="18915" windowHeight="8325" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -5103,8 +5103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6623,8 +6623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se publica por consola el resultado de la búsqueda del CBR
</commit_message>
<xml_diff>
--- a/cbr/modelo/speedcraft-casos.xlsx
+++ b/cbr/modelo/speedcraft-casos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="285" windowWidth="18915" windowHeight="8325" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="18915" windowHeight="8265" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -5103,8 +5103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6623,7 +6623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Añado la lógica del juego de aplicación del cbr
</commit_message>
<xml_diff>
--- a/cbr/modelo/speedcraft-casos.xlsx
+++ b/cbr/modelo/speedcraft-casos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="18915" windowHeight="8265" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="465" windowWidth="18915" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1629,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:T85"/>
   <sheetViews>
-    <sheetView topLeftCell="M75" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58:T85"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3563,7 +3563,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:S28"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5103,7 +5103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
@@ -6624,7 +6624,7 @@
   <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se implementan la configuración de acuerdo con el resultado de la búsqueda CBR
</commit_message>
<xml_diff>
--- a/cbr/modelo/speedcraft-casos.xlsx
+++ b/cbr/modelo/speedcraft-casos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="465" windowWidth="18915" windowHeight="8145"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="18915" windowHeight="8085" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1629,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:T85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3562,7 +3562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -5103,8 +5103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="N17" workbookViewId="0">
+      <selection activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6616,6 +6616,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Actualizar casos para varios almacenes
</commit_message>
<xml_diff>
--- a/cbr/modelo/speedcraft-casos.xlsx
+++ b/cbr/modelo/speedcraft-casos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="18915" windowHeight="8085" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="18915" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -997,16 +997,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>253512</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>45427</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>714300</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>91512</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>85648</xdr:rowOff>
+      <xdr:rowOff>92975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1023,7 +1023,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="876300" y="5181600"/>
+          <a:off x="3550627" y="5188927"/>
           <a:ext cx="600000" cy="619048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1042,7 +1042,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>62935</xdr:colOff>
+      <xdr:colOff>62936</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>95173</xdr:rowOff>
     </xdr:to>
@@ -1074,15 +1074,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>98181</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>54952</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>38758</xdr:colOff>
+      <xdr:colOff>60738</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>76125</xdr:rowOff>
+      <xdr:rowOff>83452</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1099,7 +1099,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2362200" y="5191125"/>
+          <a:off x="2252296" y="5198452"/>
           <a:ext cx="600000" cy="600000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1156,7 +1156,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>151591</xdr:colOff>
+      <xdr:colOff>151592</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>66600</xdr:rowOff>
     </xdr:to>
@@ -1226,15 +1226,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>51858</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>61384</xdr:rowOff>
+      <xdr:colOff>183742</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>141980</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>104025</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>23283</xdr:rowOff>
+      <xdr:colOff>235909</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>103879</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1251,8 +1251,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1173691" y="632884"/>
-          <a:ext cx="2469238" cy="1295399"/>
+          <a:off x="564742" y="2427980"/>
+          <a:ext cx="2462725" cy="1295399"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1263,16 +1263,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>60325</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>82306</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>60324</xdr:rowOff>
+      <xdr:rowOff>1708</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>86179</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>22224</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>562429</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>154108</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1289,8 +1289,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1182158" y="1965324"/>
-          <a:ext cx="2442925" cy="1295400"/>
+          <a:off x="4141421" y="1906708"/>
+          <a:ext cx="2436412" cy="1295400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1301,16 +1301,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>55032</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>642327</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>128301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>95730</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>21165</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>366826</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>94434</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1327,8 +1327,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1185333" y="3293532"/>
-          <a:ext cx="2449301" cy="1299633"/>
+          <a:off x="3939442" y="3557301"/>
+          <a:ext cx="2442788" cy="1299633"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1629,13 +1629,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:T85"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="E76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
@@ -5103,7 +5103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N17" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>

</xml_diff>